<commit_message>
Cleaned up minor copying error
</commit_message>
<xml_diff>
--- a/Excel_Challenge_578 - Find Maximum Product.xlsx
+++ b/Excel_Challenge_578 - Find Maximum Product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA9C9F-6739-46C7-A496-407D34DA651A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A37EC9-2EB2-465D-95A9-6F8B8DB6DC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23790" yWindow="0" windowWidth="23880" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1298,6 +1298,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -5619,8 +5622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7609F94-D06D-46DE-9604-3FD5C8A48854}">
   <dimension ref="A1:S743"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N69" sqref="N69"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5639,7 +5642,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -6267,7 +6270,7 @@
         <v>-41-32-29</v>
       </c>
     </row>
-    <row r="35" spans="2:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <v>10-19-6</v>
       </c>
@@ -10198,9 +10201,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N1" r:id="rId1" xr:uid="{39E413D4-070A-4592-B58D-958086F05055}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>